<commit_message>
Check if not before/after dates are less then 3 characters and if yes add 0 & clear map_points.json
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/seals.xlsx
+++ b/ExcelToXMLConverter/resources/seals.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="709">
   <si>
     <t xml:space="preserve">TITLE</t>
   </si>
@@ -1037,6 +1037,9 @@
     <t xml:space="preserve">42.840833, 23.371111</t>
   </si>
   <si>
+    <t xml:space="preserve">42.840833, 23.371113</t>
+  </si>
+  <si>
     <t xml:space="preserve">42.5569, 27.6405</t>
   </si>
   <si>
@@ -1047,6 +1050,9 @@
   </si>
   <si>
     <t xml:space="preserve">42.546054, 22.962896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42.840833, 23.371181</t>
   </si>
   <si>
     <t xml:space="preserve">FIND DATE</t>
@@ -2337,7 +2343,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2372,6 +2378,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -2470,7 +2482,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2539,19 +2551,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2634,8 +2654,8 @@
   </sheetPr>
   <dimension ref="A1:Z131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z15" activeCellId="0" sqref="Z15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z66" activeCellId="0" sqref="Z66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6180,7 +6200,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>330</v>
       </c>
@@ -6214,22 +6234,28 @@
       <c r="N66" s="5" t="s">
         <v>336</v>
       </c>
+      <c r="P66" s="17" t="s">
+        <v>338</v>
+      </c>
       <c r="S66" s="5" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="T66" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="U66" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="X66" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
+      </c>
+      <c r="Z66" s="18" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -6237,10 +6263,10 @@
         <v>2005</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J67" s="5" t="n">
         <v>1912</v>
@@ -6262,528 +6288,528 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="L70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="N70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="O70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="P70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="Q70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="R70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="S70" s="5" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="T70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="U70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="V70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="W70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="X70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="Y70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="Z70" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="I71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="L71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="N71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="O71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="Q71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="R71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="T71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="U71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="V71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="W71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="X71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="Y71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="Z71" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="L72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="N72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="O72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="Q72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="R72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="S72" s="5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="T72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="U72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="V72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="W72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="X72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="Y72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="Z72" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="H73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="L73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="M73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="N73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="O73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="P73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="Q73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="R73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="S73" s="5" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="T73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="U73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="V73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="W73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="X73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="Y73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="Z73" s="8" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="N74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="O74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="R74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="S74" s="5" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="T74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="U74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="V74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="W74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="X74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="Y74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="Z74" s="8" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="L75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="M75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="N75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="O75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="P75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="Q75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="R75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="S75" s="5" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="T75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="U75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="V75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="W75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="X75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="Y75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="Z75" s="15" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="14" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B76" s="11"/>
       <c r="F76" s="4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="T76" s="8" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="U76" s="8"/>
       <c r="V76" s="8"/>
@@ -6794,97 +6820,97 @@
     </row>
     <row r="77" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="L77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="M77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="N77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="O77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="P77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="Q77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="R77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="S77" s="5" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="T77" s="15" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="U77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="V77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="W77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="X77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="Y77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="Z77" s="15" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B80" s="11" t="n">
         <v>182</v>
@@ -6964,177 +6990,177 @@
     </row>
     <row r="81" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M81" s="5" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="N81" s="5" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="S81" s="5" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="U81" s="8" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="V81" s="8"/>
       <c r="W81" s="8" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="X81" s="8"/>
       <c r="Y81" s="8" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="Z81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="N82" s="5" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="S82" s="5" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="U82" s="8" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="V82" s="8"/>
       <c r="W82" s="8" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="X82" s="8"/>
       <c r="Y82" s="8" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="Z82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U83" s="6" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="W83" s="6" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="X83" s="6" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="Z83" s="6" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F84" s="11"/>
       <c r="G84" s="4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="U84" s="6" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="W84" s="6" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="X84" s="6" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="Z84" s="6" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="357" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N85" s="5" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="O85" s="5" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="U85" s="6" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="U86" s="8" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="V86" s="8"/>
       <c r="W86" s="8"/>
@@ -7144,28 +7170,28 @@
     </row>
     <row r="87" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>183</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>183</v>
@@ -7180,13 +7206,13 @@
         <v>183</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="O87" s="5" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="P87" s="5" t="s">
         <v>183</v>
@@ -7201,7 +7227,7 @@
         <v>183</v>
       </c>
       <c r="T87" s="8" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="U87" s="8" t="s">
         <v>183</v>
@@ -7219,33 +7245,33 @@
         <v>183</v>
       </c>
       <c r="Z87" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>190</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>190</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="I88" s="5" t="s">
         <v>190</v>
@@ -7266,7 +7292,7 @@
         <v>119</v>
       </c>
       <c r="O88" s="5" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="P88" s="5" t="s">
         <v>190</v>
@@ -7281,7 +7307,7 @@
         <v>190</v>
       </c>
       <c r="T88" s="8" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="U88" s="8" t="s">
         <v>190</v>
@@ -7299,12 +7325,12 @@
         <v>190</v>
       </c>
       <c r="Z88" s="8" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B89" s="11" t="n">
         <v>30</v>
@@ -7366,299 +7392,299 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="I92" s="5" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="L92" s="5" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="M92" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="N92" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q92" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="R92" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="N92" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="P92" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q92" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="R92" s="5" t="s">
-        <v>442</v>
-      </c>
       <c r="S92" s="5" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="U92" s="6" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="V92" s="6" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="W92" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="X92" s="6" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="Y92" s="6" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="Z92" s="8" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="I93" s="5" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="Q93" s="5" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="R93" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="U93" s="6" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="V93" s="6" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="W93" s="6" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="X93" s="6" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="Y93" s="6" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="Z93" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="L96" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="M96" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="N96" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="O96" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="P96" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q96" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="R96" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="S96" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="T96" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="U96" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="M96" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="N96" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="O96" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="P96" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q96" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="R96" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="S96" s="5" t="s">
+      <c r="V96" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="W96" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="T96" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="U96" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="V96" s="8" t="s">
-        <v>468</v>
-      </c>
-      <c r="W96" s="8" t="s">
-        <v>469</v>
-      </c>
       <c r="X96" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="Y96" s="8" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="Z96" s="8" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="H97" s="5" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="L97" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="M97" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="N97" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="O97" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="P97" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q97" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="R97" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="S97" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="T97" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="U97" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="V97" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="M97" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="N97" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="O97" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="P97" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="Q97" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="R97" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="S97" s="5" t="s">
+      <c r="W97" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="T97" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="U97" s="8" t="s">
-        <v>478</v>
-      </c>
-      <c r="V97" s="8" t="s">
-        <v>474</v>
-      </c>
-      <c r="W97" s="8" t="s">
-        <v>475</v>
-      </c>
       <c r="X97" s="8" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="Y97" s="8" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="Z97" s="8" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="14" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B98" s="11" t="n">
         <v>30</v>
@@ -7714,277 +7740,277 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="I105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="K105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="L105" s="5" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="M105" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="N105" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="N105" s="5" t="s">
-        <v>487</v>
-      </c>
       <c r="O105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="P105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="Q105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="R105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="S105" s="5" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="T105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="U105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="V105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="W105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="X105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="Y105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="Z105" s="8" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="I106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="K106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="L106" s="5" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="M106" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="N106" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="N106" s="5" t="s">
-        <v>491</v>
-      </c>
       <c r="O106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="P106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="Q106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="R106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="S106" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="T106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="U106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="V106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="W106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="X106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="Y106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="Z106" s="8" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="I107" s="5" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="J107" s="5" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="K107" s="5" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="L107" s="5" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="M107" s="5" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="N107" s="5" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="O107" s="5" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="P107" s="5" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="Q107" s="5" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="R107" s="5" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="S107" s="5" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="T107" s="6" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="U107" s="6" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="V107" s="6" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="W107" s="6" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="X107" s="6" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="Y107" s="6" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="Z107" s="6" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>1</v>
@@ -8041,7 +8067,7 @@
         <v>18</v>
       </c>
       <c r="T108" s="6" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="U108" s="6" t="s">
         <v>20</v>
@@ -8064,87 +8090,87 @@
     </row>
     <row r="109" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="I109" s="5" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="J109" s="5" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="K109" s="5" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="L109" s="5" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="M109" s="5" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="N109" s="5" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="O109" s="5" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="P109" s="5" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="Q109" s="5" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="R109" s="5" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="S109" s="5" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="T109" s="6" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="U109" s="6" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="V109" s="6" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="W109" s="6" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="X109" s="6" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="Y109" s="6" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="Z109" s="6" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>1</v>
@@ -8201,7 +8227,7 @@
         <v>18</v>
       </c>
       <c r="T110" s="6" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="U110" s="6" t="s">
         <v>20</v>
@@ -8224,292 +8250,292 @@
     </row>
     <row r="111" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="I111" s="5" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="J111" s="5" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="K111" s="5" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="L111" s="5" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="M111" s="5" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="N111" s="5" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="O111" s="5" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="P111" s="5" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="Q111" s="5" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="R111" s="5" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="S111" s="5" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="T111" s="8" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="U111" s="8" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="V111" s="8" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="W111" s="8" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="X111" s="8" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="Y111" s="8" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="Z111" s="8" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="J112" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="K112" s="5" t="s">
+        <v>561</v>
+      </c>
+      <c r="L112" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="N112" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="O112" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="P112" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q112" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="R112" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="S112" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="T112" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="U112" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="V112" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="W112" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="X112" s="8" t="s">
+        <v>574</v>
+      </c>
+      <c r="Y112" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="Z112" s="8" t="s">
         <v>576</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="G112" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="H112" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="I112" s="5" t="s">
-        <v>557</v>
-      </c>
-      <c r="J112" s="5" t="s">
-        <v>558</v>
-      </c>
-      <c r="K112" s="5" t="s">
-        <v>559</v>
-      </c>
-      <c r="L112" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="M112" s="5" t="s">
-        <v>561</v>
-      </c>
-      <c r="N112" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="O112" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="P112" s="5" t="s">
-        <v>564</v>
-      </c>
-      <c r="Q112" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="R112" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="S112" s="5" t="s">
-        <v>567</v>
-      </c>
-      <c r="T112" s="8" t="s">
-        <v>568</v>
-      </c>
-      <c r="U112" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="V112" s="8" t="s">
-        <v>570</v>
-      </c>
-      <c r="W112" s="8" t="s">
-        <v>571</v>
-      </c>
-      <c r="X112" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="Y112" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="Z112" s="8" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="L113" s="5" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="M113" s="5" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="N113" s="5" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="P113" s="5" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="Q113" s="5" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="R113" s="5" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="S113" s="5" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="J115" s="5" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="L115" s="5" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="N115" s="5" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="O115" s="5" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="T115" s="6" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="U115" s="6" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="V115" s="6" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="267.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="J116" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="L116" s="5" t="s">
+        <v>597</v>
+      </c>
+      <c r="N116" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="O116" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="T116" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="U116" s="6" t="s">
         <v>601</v>
       </c>
-      <c r="D116" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="J116" s="5" t="s">
-        <v>594</v>
-      </c>
-      <c r="L116" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="N116" s="5" t="s">
-        <v>596</v>
-      </c>
-      <c r="O116" s="5" t="s">
-        <v>597</v>
-      </c>
-      <c r="T116" s="6" t="s">
-        <v>602</v>
-      </c>
-      <c r="U116" s="6" t="s">
-        <v>599</v>
-      </c>
       <c r="V116" s="6" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="M117" s="5" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="U117" s="6" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="V117" s="6" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="W117" s="15"/>
       <c r="X117" s="15"/>
@@ -8518,330 +8544,330 @@
     </row>
     <row r="118" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="W118" s="8"/>
       <c r="X118" s="8"/>
       <c r="Y118" s="8"/>
       <c r="Z118" s="8" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="153" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="J119" s="5" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="K119" s="5" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="L119" s="5" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="M119" s="5" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="N119" s="5" t="s">
-        <v>625</v>
-      </c>
-      <c r="O119" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
+      </c>
+      <c r="O119" s="19" t="s">
+        <v>628</v>
       </c>
       <c r="P119" s="5" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="Q119" s="5" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="R119" s="5" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="S119" s="5" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="B120" s="18" t="s">
-        <v>632</v>
-      </c>
-      <c r="C120" s="18" t="s">
         <v>633</v>
       </c>
-      <c r="D120" s="19" t="s">
+      <c r="B120" s="20" t="s">
         <v>634</v>
       </c>
-      <c r="E120" s="20" t="s">
+      <c r="C120" s="20" t="s">
         <v>635</v>
       </c>
-      <c r="F120" s="20" t="s">
+      <c r="D120" s="21" t="s">
         <v>636</v>
       </c>
-      <c r="G120" s="20" t="s">
+      <c r="E120" s="22" t="s">
         <v>637</v>
       </c>
-      <c r="H120" s="19" t="s">
+      <c r="F120" s="22" t="s">
         <v>638</v>
       </c>
-      <c r="I120" s="19" t="s">
+      <c r="G120" s="22" t="s">
         <v>639</v>
       </c>
-      <c r="J120" s="19" t="s">
+      <c r="H120" s="21" t="s">
         <v>640</v>
       </c>
-      <c r="K120" s="19" t="s">
+      <c r="I120" s="21" t="s">
         <v>641</v>
       </c>
-      <c r="L120" s="19" t="s">
+      <c r="J120" s="21" t="s">
         <v>642</v>
       </c>
+      <c r="K120" s="21" t="s">
+        <v>643</v>
+      </c>
+      <c r="L120" s="21" t="s">
+        <v>644</v>
+      </c>
       <c r="M120" s="5" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="N120" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="O120" s="19" t="s">
-        <v>645</v>
-      </c>
-      <c r="P120" s="19" t="s">
         <v>646</v>
       </c>
-      <c r="Q120" s="19" t="s">
+      <c r="O120" s="21" t="s">
         <v>647</v>
       </c>
-      <c r="R120" s="19" t="s">
+      <c r="P120" s="21" t="s">
         <v>648</v>
       </c>
-      <c r="S120" s="19" t="s">
+      <c r="Q120" s="21" t="s">
         <v>649</v>
+      </c>
+      <c r="R120" s="21" t="s">
+        <v>650</v>
+      </c>
+      <c r="S120" s="21" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="H123" s="5" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="J123" s="5" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="K123" s="5" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="L123" s="5" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="M123" s="5" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="N123" s="5" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="O123" s="5" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="P123" s="5" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="Q123" s="5" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="R123" s="5" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="S123" s="5" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="H124" s="5" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="I124" s="5" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="J124" s="5" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="K124" s="5" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="L124" s="5" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="M124" s="5" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="N124" s="5" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="O124" s="5" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="P124" s="5" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="Q124" s="5" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="R124" s="5" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="S124" s="5" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="L125" s="5" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="M125" s="5" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="P125" s="5" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="R125" s="5" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="S125" s="5" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="R126" s="5" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="S126" s="5" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>

</xml_diff>